<commit_message>
Added equations of best fit to the xlsx
</commit_message>
<xml_diff>
--- a/putty_output/cybot4graphs.xlsx
+++ b/putty_output/cybot4graphs.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\cpre288\288-lab\putty_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63B2750-277A-4437-81B1-64F8A0567FD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89D2A1D-FD16-4A85-BE91-9879F0E8E2EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cybot40305073643" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">cybot40305073643!$A$1:$A$33</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">cybot40305073643!$B$1:$B$33</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">cybot40305073643!$A$1:$A$33</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">cybot40305073643!$B$1:$B$33</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -638,8 +644,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -723,7 +729,250 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.4993104675474889E-3"/>
+                  <c:y val="-0.57529115419086962"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>y = -9E-06x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>5</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> + 0.0024x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>4</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> - 0.2432x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> + 12.399x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent5"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> - 328.82x + 4571.2</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.9503981493838694E-2"/>
+                  <c:y val="-0.50884073243304084"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="accent6"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>y = 2447e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000">
+                        <a:solidFill>
+                          <a:schemeClr val="accent6"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>-0.024x</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:endParaRPr>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>cybot40305073643!$A$1:$A$33</c:f>
               <c:numCache>
@@ -830,8 +1079,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>cybot40305073643!$B$1:$B$33</c:f>
               <c:numCache>
@@ -938,8 +1187,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9469-4CFB-BC64-7574546F1262}"/>
@@ -955,13 +1204,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
         <c:axId val="1907523311"/>
         <c:axId val="2087489215"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
+            <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="0"/>
                 <c:order val="0"/>
@@ -975,7 +1222,17 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:marker>
-                  <c:symbol val="none"/>
+                  <c:symbol val="circle"/>
+                  <c:size val="17"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
                 </c:marker>
                 <c:dLbls>
                   <c:spPr>
@@ -1031,7 +1288,7 @@
                     </c:ext>
                   </c:extLst>
                 </c:dLbls>
-                <c:cat>
+                <c:xVal>
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1144,8 +1401,8 @@
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
-                </c:cat>
-                <c:val>
+                </c:xVal>
+                <c:yVal>
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1258,19 +1515,19 @@
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
+                </c:yVal>
+                <c:smooth val="1"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-9469-4CFB-BC64-7574546F1262}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
-            </c15:filteredLineSeries>
+            </c15:filteredScatterSeries>
           </c:ext>
         </c:extLst>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1907523311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1371,11 +1628,8 @@
         </c:txPr>
         <c:crossAx val="2087489215"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="2087489215"/>
         <c:scaling>
@@ -1497,7 +1751,7 @@
         </c:txPr>
         <c:crossAx val="1907523311"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2179,16 +2433,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2516,7 +2770,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final commit tonight, touched up excel graph
</commit_message>
<xml_diff>
--- a/putty_output/cybot4graphs.xlsx
+++ b/putty_output/cybot4graphs.xlsx
@@ -8,19 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\cpre288\288-lab\putty_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89D2A1D-FD16-4A85-BE91-9879F0E8E2EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EB975F-8630-44B3-87FB-08DA58D147FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cybot40305073643" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">cybot40305073643!$A$1:$A$33</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">cybot40305073643!$B$1:$B$33</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">cybot40305073643!$A$1:$A$33</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">cybot40305073643!$B$1:$B$33</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -648,15 +642,12 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>ADC Reading</c:v>
-          </c:tx>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -667,7 +658,7 @@
             <c:size val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -710,7 +701,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -733,215 +724,21 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.4993104675474889E-3"/>
-                  <c:y val="-0.57529115419086962"/>
+                  <c:x val="-4.8304258577847259E-2"/>
+                  <c:y val="-0.5614985887901297"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>y = -9E-06x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>5</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t> + 0.0024x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>4</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t> - 0.2432x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>3</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t> + 12.399x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>2</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent5"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t> - 328.82x + 4571.2</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:solidFill>
-                    <a:schemeClr val="bg1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.9503981493838694E-2"/>
-                  <c:y val="-0.50884073243304084"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="accent6"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>y = 2447e</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="accent6"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>-0.024x</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6"/>
-                      </a:solidFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -979,103 +776,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3862</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3421</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>2585</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>2277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>1892</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>1779</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>1702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>1701</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17</c:v>
+                  <c:v>1559</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>1491</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19</c:v>
+                  <c:v>1423</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>1399</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>1323</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22</c:v>
+                  <c:v>1256</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23</c:v>
+                  <c:v>1207</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24</c:v>
+                  <c:v>1185</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>1139</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26</c:v>
+                  <c:v>1114</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29</c:v>
+                  <c:v>1023</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30</c:v>
+                  <c:v>999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32</c:v>
+                  <c:v>951</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35</c:v>
+                  <c:v>884</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>40</c:v>
+                  <c:v>819</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>45</c:v>
+                  <c:v>730</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>50</c:v>
+                  <c:v>680</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>55</c:v>
+                  <c:v>635</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>60</c:v>
+                  <c:v>606</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>65</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>70</c:v>
+                  <c:v>536</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>75</c:v>
+                  <c:v>509</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>80</c:v>
+                  <c:v>486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1087,111 +884,111 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>3862</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3421</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2585</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2277</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2003</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1892</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1779</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1702</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1701</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1630</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1559</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1491</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1423</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1399</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1323</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1256</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1207</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1185</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1139</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1114</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1023</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>999</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>951</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>884</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>819</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>730</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>680</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>635</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>606</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>555</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>536</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>509</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>486</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9469-4CFB-BC64-7574546F1262}"/>
+              <c16:uniqueId val="{00000000-9469-4CFB-BC64-7574546F1262}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1206,326 +1003,7 @@
         </c:dLbls>
         <c:axId val="1907523311"/>
         <c:axId val="2087489215"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:spPr>
-                  <a:ln w="31750" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="17"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="lt1"/>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="ctr"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525">
-                            <a:solidFill>
-                              <a:schemeClr val="dk1">
-                                <a:lumMod val="50000"/>
-                                <a:lumOff val="50000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>cybot40305073643!$A$1:$A$33</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="33"/>
-                      <c:pt idx="0">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>18</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>19</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>20</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>21</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>23</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>24</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>25</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>26</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>30</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>32</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>35</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>40</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>45</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>50</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>55</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>60</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>65</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>70</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>75</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>80</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>cybot40305073643!$A$1:$A$33</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="33"/>
-                      <c:pt idx="0">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>12</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>18</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>19</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>20</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>21</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>23</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>24</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>25</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>26</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>30</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>32</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>35</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>40</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>45</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>50</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>55</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>60</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>65</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>70</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>75</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>80</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="1"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-9469-4CFB-BC64-7574546F1262}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1907523311"/>
@@ -2433,13 +1911,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2770,273 +2248,273 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>3862</v>
+      </c>
+      <c r="B1">
         <v>2</v>
-      </c>
-      <c r="B1">
-        <v>3862</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>3421</v>
+      </c>
+      <c r="B2">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>3421</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2585</v>
+      </c>
+      <c r="B3">
         <v>8</v>
-      </c>
-      <c r="B3">
-        <v>2585</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2277</v>
+      </c>
+      <c r="B4">
         <v>10</v>
-      </c>
-      <c r="B4">
-        <v>2277</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>2003</v>
+      </c>
+      <c r="B5">
         <v>12</v>
-      </c>
-      <c r="B5">
-        <v>2003</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>1892</v>
+      </c>
+      <c r="B6">
         <v>13</v>
-      </c>
-      <c r="B6">
-        <v>1892</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>1779</v>
+      </c>
+      <c r="B7">
         <v>14</v>
-      </c>
-      <c r="B7">
-        <v>1779</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>1702</v>
+      </c>
+      <c r="B8">
         <v>15</v>
-      </c>
-      <c r="B8">
-        <v>1702</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>1701</v>
+      </c>
+      <c r="B9">
         <v>15</v>
-      </c>
-      <c r="B9">
-        <v>1701</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>1630</v>
+      </c>
+      <c r="B10">
         <v>16</v>
-      </c>
-      <c r="B10">
-        <v>1630</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>1559</v>
+      </c>
+      <c r="B11">
         <v>17</v>
-      </c>
-      <c r="B11">
-        <v>1559</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>1491</v>
+      </c>
+      <c r="B12">
         <v>18</v>
-      </c>
-      <c r="B12">
-        <v>1491</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>1423</v>
+      </c>
+      <c r="B13">
         <v>19</v>
-      </c>
-      <c r="B13">
-        <v>1423</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>1399</v>
+      </c>
+      <c r="B14">
         <v>20</v>
-      </c>
-      <c r="B14">
-        <v>1399</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>1323</v>
+      </c>
+      <c r="B15">
         <v>21</v>
-      </c>
-      <c r="B15">
-        <v>1323</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>1256</v>
+      </c>
+      <c r="B16">
         <v>22</v>
-      </c>
-      <c r="B16">
-        <v>1256</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>1207</v>
+      </c>
+      <c r="B17">
         <v>23</v>
-      </c>
-      <c r="B17">
-        <v>1207</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>1185</v>
+      </c>
+      <c r="B18">
         <v>24</v>
-      </c>
-      <c r="B18">
-        <v>1185</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>1139</v>
+      </c>
+      <c r="B19">
         <v>25</v>
-      </c>
-      <c r="B19">
-        <v>1139</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>1114</v>
+      </c>
+      <c r="B20">
         <v>26</v>
-      </c>
-      <c r="B20">
-        <v>1114</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>1023</v>
+      </c>
+      <c r="B21">
         <v>29</v>
-      </c>
-      <c r="B21">
-        <v>1023</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>999</v>
+      </c>
+      <c r="B22">
         <v>30</v>
-      </c>
-      <c r="B22">
-        <v>999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>951</v>
+      </c>
+      <c r="B23">
         <v>32</v>
-      </c>
-      <c r="B23">
-        <v>951</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>884</v>
+      </c>
+      <c r="B24">
         <v>35</v>
-      </c>
-      <c r="B24">
-        <v>884</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>819</v>
+      </c>
+      <c r="B25">
         <v>40</v>
-      </c>
-      <c r="B25">
-        <v>819</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>730</v>
+      </c>
+      <c r="B26">
         <v>45</v>
-      </c>
-      <c r="B26">
-        <v>730</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
+        <v>680</v>
+      </c>
+      <c r="B27">
         <v>50</v>
-      </c>
-      <c r="B27">
-        <v>680</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>635</v>
+      </c>
+      <c r="B28">
         <v>55</v>
-      </c>
-      <c r="B28">
-        <v>635</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>606</v>
+      </c>
+      <c r="B29">
         <v>60</v>
-      </c>
-      <c r="B29">
-        <v>606</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>555</v>
+      </c>
+      <c r="B30">
         <v>65</v>
-      </c>
-      <c r="B30">
-        <v>555</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>536</v>
+      </c>
+      <c r="B31">
         <v>70</v>
-      </c>
-      <c r="B31">
-        <v>536</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>509</v>
+      </c>
+      <c r="B32">
         <v>75</v>
-      </c>
-      <c r="B32">
-        <v>509</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>486</v>
+      </c>
+      <c r="B33">
         <v>80</v>
-      </c>
-      <c r="B33">
-        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>